<commit_message>
TC-36868 MTR-2463 MTR-2464 added
</commit_message>
<xml_diff>
--- a/src/test/resources/testdata/VOLDP1.xlsx
+++ b/src/test/resources/testdata/VOLDP1.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20403"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E1FA1A4F-CAA5-42FF-B843-93689DB48CBA}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F0A607C-4AF5-4CC9-9E6A-A9ED7F91F394}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="171" uniqueCount="36">
   <si>
     <t>FirstName</t>
   </si>
@@ -121,16 +121,13 @@
     <t>Economy</t>
   </si>
   <si>
-    <t>Standard</t>
-  </si>
-  <si>
     <t>Annual</t>
   </si>
   <si>
-    <t>11012023</t>
-  </si>
-  <si>
-    <t>2023</t>
+    <t>2020</t>
+  </si>
+  <si>
+    <t>04012023</t>
   </si>
 </sst>
 </file>
@@ -469,10 +466,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:P8"/>
+  <dimension ref="A1:P11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+      <selection activeCell="I10" sqref="I10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -570,10 +567,10 @@
         <v>22</v>
       </c>
       <c r="M2" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="N2" s="6" t="s">
         <v>34</v>
-      </c>
-      <c r="N2" s="6" t="s">
-        <v>36</v>
       </c>
       <c r="O2" s="6" t="s">
         <v>31</v>
@@ -620,16 +617,16 @@
         <v>22</v>
       </c>
       <c r="M3" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="N3" s="6" t="s">
         <v>34</v>
-      </c>
-      <c r="N3" s="6" t="s">
-        <v>36</v>
       </c>
       <c r="O3" s="6" t="s">
         <v>31</v>
       </c>
       <c r="P3" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="4" spans="1:16" s="3" customFormat="1" ht="21" x14ac:dyDescent="0.4">
@@ -670,10 +667,10 @@
         <v>22</v>
       </c>
       <c r="M4" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="N4" s="6" t="s">
         <v>34</v>
-      </c>
-      <c r="N4" s="6" t="s">
-        <v>36</v>
       </c>
       <c r="O4" s="6" t="s">
         <v>31</v>
@@ -720,16 +717,16 @@
         <v>22</v>
       </c>
       <c r="M5" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="N5" s="6" t="s">
         <v>34</v>
-      </c>
-      <c r="N5" s="6" t="s">
-        <v>36</v>
       </c>
       <c r="O5" s="6" t="s">
         <v>31</v>
       </c>
       <c r="P5" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="6" spans="1:16" s="3" customFormat="1" ht="21" x14ac:dyDescent="0.4">
@@ -770,10 +767,10 @@
         <v>22</v>
       </c>
       <c r="M6" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="N6" s="6" t="s">
         <v>34</v>
-      </c>
-      <c r="N6" s="6" t="s">
-        <v>36</v>
       </c>
       <c r="O6" s="6" t="s">
         <v>31</v>
@@ -820,16 +817,16 @@
         <v>22</v>
       </c>
       <c r="M7" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="N7" s="6" t="s">
         <v>34</v>
-      </c>
-      <c r="N7" s="6" t="s">
-        <v>36</v>
       </c>
       <c r="O7" s="6" t="s">
         <v>31</v>
       </c>
       <c r="P7" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="8" spans="1:16" s="3" customFormat="1" ht="21" x14ac:dyDescent="0.4">
@@ -870,15 +867,165 @@
         <v>22</v>
       </c>
       <c r="M8" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="N8" s="6" t="s">
         <v>34</v>
-      </c>
-      <c r="N8" s="6" t="s">
-        <v>36</v>
       </c>
       <c r="O8" s="6" t="s">
         <v>31</v>
       </c>
       <c r="P8" s="3" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="9" spans="1:16" s="3" customFormat="1" ht="21" x14ac:dyDescent="0.4">
+      <c r="A9" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="E9" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="F9" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="G9" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="H9" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="I9" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="J9" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="K9" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="L9" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="M9" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="N9" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="O9" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="P9" s="3" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="10" spans="1:16" s="3" customFormat="1" ht="21" x14ac:dyDescent="0.4">
+      <c r="A10" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C10" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E10" s="5">
+        <v>33837</v>
+      </c>
+      <c r="F10" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="G10" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="H10" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="I10" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="J10" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="K10" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="L10" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="M10" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="N10" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="O10" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="P10" s="3" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="11" spans="1:16" s="3" customFormat="1" ht="21" x14ac:dyDescent="0.4">
+      <c r="A11" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C11" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="E11" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="F11" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="G11" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="H11" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="I11" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="J11" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="K11" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="L11" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="M11" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="N11" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="O11" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="P11" s="3" t="s">
         <v>32</v>
       </c>
     </row>

</xml_diff>